<commit_message>
A72 A73 調整加入 WT & Default
</commit_message>
<xml_diff>
--- a/Transfer/FileDownloads/A73.xlsx
+++ b/Transfer/FileDownloads/A73.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>TM</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>Ca-C</t>
+  </si>
+  <si>
+    <t>WT</t>
   </si>
 </sst>
 </file>
@@ -444,7 +447,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -594,6 +597,22 @@
         <v>25.818000000000001</v>
       </c>
     </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>0.52716666666666701</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>